<commit_message>
Assignment 6 and quiz 4
</commit_message>
<xml_diff>
--- a/Home/JaroneJabonillo_PSP_42825.xlsx
+++ b/Home/JaroneJabonillo_PSP_42825.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="999" uniqueCount="70">
   <si>
     <t>Student</t>
   </si>
@@ -231,6 +231,15 @@
   </si>
   <si>
     <t>These programs include recursion version of the previous assignments. It uses recursion in order to calculate exponents of a value as well as the GCD of two given values. The assignment really helped me to review recursion and I had to use Euclid's Algorithm to create recursion for the GCD. Overall it was good practice.</t>
+  </si>
+  <si>
+    <t>Fractions</t>
+  </si>
+  <si>
+    <t>Assignment #6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Within this class is the Fractions class, a driver, as well as a unit test file for the class. During this exercise, I was able to review classes and learn how to utilize netbean's java utility test program. I found the program to be very helpful in creating and debugging classes. </t>
   </si>
 </sst>
 </file>
@@ -2828,12 +2837,12 @@
       </c>
       <c r="F7" s="1">
         <f>Assignment9!H7</f>
-        <v>0</v>
+        <v>316</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="1">
         <f t="shared" ref="H7:H10" si="0">E7+F7</f>
-        <v>0</v>
+        <v>316</v>
       </c>
       <c r="J7" s="33" t="s">
         <v>37</v>
@@ -2861,12 +2870,12 @@
       </c>
       <c r="F8" s="1">
         <f>Assignment9!H8</f>
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="J8" s="36"/>
       <c r="K8" s="37"/>
@@ -2926,12 +2935,12 @@
       </c>
       <c r="F10" s="1">
         <f>Assignment9!H10</f>
-        <v>1059</v>
+        <v>1235</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="1">
         <f t="shared" si="0"/>
-        <v>1059</v>
+        <v>1235</v>
       </c>
       <c r="J10" s="36"/>
       <c r="K10" s="37"/>
@@ -2991,12 +3000,12 @@
       </c>
       <c r="F12" s="1">
         <f>Assignment9!H12</f>
-        <v>1059</v>
+        <v>1235</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="1">
         <f t="shared" ref="H12:H13" si="1">E12+F12</f>
-        <v>1059</v>
+        <v>1235</v>
       </c>
       <c r="J12" s="36"/>
       <c r="K12" s="37"/>
@@ -3022,12 +3031,12 @@
       </c>
       <c r="F13" s="1">
         <f>Assignment9!H13</f>
-        <v>1085</v>
+        <v>1437</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="1">
         <f t="shared" si="1"/>
-        <v>1085</v>
+        <v>1437</v>
       </c>
       <c r="J13" s="33" t="s">
         <v>40</v>
@@ -3058,7 +3067,7 @@
       <c r="G14" s="3"/>
       <c r="H14" s="1">
         <f>IF($G$23&lt;&gt;0,60*H12/$G$23,"-")</f>
-        <v>99.126365054602189</v>
+        <v>83.634311512415351</v>
       </c>
       <c r="J14" s="42"/>
       <c r="K14" s="43"/>
@@ -3129,15 +3138,15 @@
       <c r="E17" s="8"/>
       <c r="F17" s="1">
         <f>Assignment9!G17</f>
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="G17" s="1">
         <f>E17+F17</f>
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="H17" s="2">
         <f t="shared" ref="H17:H22" si="2">IF($G$23&lt;&gt;0,G17/$G$23,"-")</f>
-        <v>0.11700468018720749</v>
+        <v>9.5936794582392779E-2</v>
       </c>
       <c r="J17" s="49" t="s">
         <v>48</v>
@@ -3161,15 +3170,15 @@
       <c r="E18" s="8"/>
       <c r="F18" s="1">
         <f>Assignment9!G18</f>
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="G18" s="1">
         <f t="shared" ref="G18:G22" si="3">E18+F18</f>
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="H18" s="2">
         <f t="shared" si="2"/>
-        <v>8.2683307332293288E-2</v>
+        <v>6.5462753950338598E-2</v>
       </c>
       <c r="J18" s="50"/>
       <c r="K18" s="50"/>
@@ -3191,15 +3200,15 @@
       <c r="E19" s="8"/>
       <c r="F19" s="1">
         <f>Assignment9!G19</f>
-        <v>285</v>
+        <v>435</v>
       </c>
       <c r="G19" s="1">
         <f t="shared" si="3"/>
-        <v>285</v>
+        <v>435</v>
       </c>
       <c r="H19" s="2">
         <f t="shared" si="2"/>
-        <v>0.44461778471138846</v>
+        <v>0.49097065462753953</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3212,15 +3221,15 @@
       <c r="E20" s="8"/>
       <c r="F20" s="1">
         <f>Assignment9!G20</f>
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="G20" s="1">
         <f t="shared" si="3"/>
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="H20" s="2">
         <f t="shared" si="2"/>
-        <v>0.10920436817472699</v>
+        <v>0.12415349887133183</v>
       </c>
       <c r="J20" s="51" t="s">
         <v>43</v>
@@ -3244,15 +3253,15 @@
       <c r="E21" s="8"/>
       <c r="F21" s="1">
         <f>Assignment9!G21</f>
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="G21" s="1">
         <f t="shared" si="3"/>
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="H21" s="2">
         <f t="shared" si="2"/>
-        <v>0.1482059282371295</v>
+        <v>0.14108352144469527</v>
       </c>
       <c r="J21" s="54"/>
       <c r="K21" s="55"/>
@@ -3274,15 +3283,15 @@
       <c r="E22" s="8"/>
       <c r="F22" s="1">
         <f>Assignment9!G22</f>
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="G22" s="1">
         <f t="shared" si="3"/>
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="H22" s="2">
         <f t="shared" si="2"/>
-        <v>9.8283931357254287E-2</v>
+        <v>8.2392776523702027E-2</v>
       </c>
       <c r="J22" s="54"/>
       <c r="K22" s="55"/>
@@ -3310,11 +3319,11 @@
       </c>
       <c r="F23" s="1">
         <f>SUM(F17:F22)</f>
-        <v>641</v>
+        <v>886</v>
       </c>
       <c r="G23" s="1">
         <f>SUM(G17:G22)</f>
-        <v>641</v>
+        <v>886</v>
       </c>
       <c r="H23" s="2">
         <f>SUM(H17:H22)</f>
@@ -3385,7 +3394,7 @@
       </c>
       <c r="H26" s="2">
         <f t="shared" ref="H26:H31" si="6">IF($G$32&lt;&gt;0,G26/$G$32,"-")</f>
-        <v>5.2631578947368418E-2</v>
+        <v>0.04</v>
       </c>
       <c r="J26" s="54"/>
       <c r="K26" s="55"/>
@@ -3414,7 +3423,7 @@
       </c>
       <c r="H27" s="2">
         <f t="shared" si="6"/>
-        <v>0.10526315789473684</v>
+        <v>0.08</v>
       </c>
       <c r="J27" s="54"/>
       <c r="K27" s="55"/>
@@ -3443,7 +3452,7 @@
       </c>
       <c r="H28" s="2">
         <f t="shared" si="6"/>
-        <v>0.42105263157894735</v>
+        <v>0.32</v>
       </c>
       <c r="J28" s="57"/>
       <c r="K28" s="58"/>
@@ -3472,7 +3481,7 @@
       </c>
       <c r="H29" s="2">
         <f t="shared" si="6"/>
-        <v>0.15789473684210525</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3484,15 +3493,15 @@
       <c r="E30" s="8"/>
       <c r="F30" s="1">
         <f>Assignment9!G30</f>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="G30" s="1">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="H30" s="2">
         <f t="shared" si="6"/>
-        <v>0.26315789473684209</v>
+        <v>0.44</v>
       </c>
       <c r="J30" s="20" t="s">
         <v>46</v>
@@ -3539,11 +3548,11 @@
       </c>
       <c r="F32" s="1">
         <f>SUM(F26:F31)</f>
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="G32" s="1">
         <f>SUM(G26:G31)</f>
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="H32" s="2">
         <f>SUM(H26:H31)</f>
@@ -3621,7 +3630,7 @@
       </c>
       <c r="H35" s="2">
         <f t="shared" ref="H35:H40" si="9">IF($G$41&lt;&gt;0,G35/$G$41,"-")</f>
-        <v>5.2631578947368418E-2</v>
+        <v>0.04</v>
       </c>
       <c r="J35" s="64"/>
       <c r="K35" s="65"/>
@@ -3650,7 +3659,7 @@
       </c>
       <c r="H36" s="2">
         <f t="shared" si="9"/>
-        <v>0.10526315789473684</v>
+        <v>0.08</v>
       </c>
       <c r="J36" s="64"/>
       <c r="K36" s="65"/>
@@ -3679,7 +3688,7 @@
       </c>
       <c r="H37" s="2">
         <f t="shared" si="9"/>
-        <v>0.42105263157894735</v>
+        <v>0.32</v>
       </c>
       <c r="J37" s="64"/>
       <c r="K37" s="65"/>
@@ -3708,7 +3717,7 @@
       </c>
       <c r="H38" s="2">
         <f t="shared" si="9"/>
-        <v>0.15789473684210525</v>
+        <v>0.12</v>
       </c>
       <c r="J38" s="64"/>
       <c r="K38" s="65"/>
@@ -3729,15 +3738,15 @@
       <c r="E39" s="8"/>
       <c r="F39" s="1">
         <f>Assignment9!G39</f>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="G39" s="1">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="H39" s="2">
         <f t="shared" si="9"/>
-        <v>0.26315789473684209</v>
+        <v>0.44</v>
       </c>
       <c r="J39" s="64"/>
       <c r="K39" s="65"/>
@@ -3790,11 +3799,11 @@
       </c>
       <c r="F41" s="1">
         <f>SUM(F35:F40)</f>
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="G41" s="1">
         <f>SUM(G35:G40)</f>
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="H41" s="2">
         <f>SUM(H35:H40)</f>
@@ -4100,12 +4109,12 @@
       </c>
       <c r="F7" s="1">
         <f>Assignment10!H7</f>
-        <v>0</v>
+        <v>316</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="1">
         <f t="shared" ref="H7:H10" si="0">E7+F7</f>
-        <v>0</v>
+        <v>316</v>
       </c>
       <c r="J7" s="33" t="s">
         <v>37</v>
@@ -4133,12 +4142,12 @@
       </c>
       <c r="F8" s="1">
         <f>Assignment10!H8</f>
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="J8" s="36"/>
       <c r="K8" s="37"/>
@@ -4198,12 +4207,12 @@
       </c>
       <c r="F10" s="1">
         <f>Assignment10!H10</f>
-        <v>1059</v>
+        <v>1235</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="1">
         <f t="shared" si="0"/>
-        <v>1059</v>
+        <v>1235</v>
       </c>
       <c r="J10" s="36"/>
       <c r="K10" s="37"/>
@@ -4263,12 +4272,12 @@
       </c>
       <c r="F12" s="1">
         <f>Assignment10!H12</f>
-        <v>1059</v>
+        <v>1235</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="1">
         <f t="shared" ref="H12:H13" si="1">E12+F12</f>
-        <v>1059</v>
+        <v>1235</v>
       </c>
       <c r="J12" s="36"/>
       <c r="K12" s="37"/>
@@ -4294,12 +4303,12 @@
       </c>
       <c r="F13" s="1">
         <f>Assignment10!H13</f>
-        <v>1085</v>
+        <v>1437</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="1">
         <f t="shared" si="1"/>
-        <v>1085</v>
+        <v>1437</v>
       </c>
       <c r="J13" s="33" t="s">
         <v>40</v>
@@ -4330,7 +4339,7 @@
       <c r="G14" s="3"/>
       <c r="H14" s="1">
         <f>IF($G$23&lt;&gt;0,60*H12/$G$23,"-")</f>
-        <v>99.126365054602189</v>
+        <v>83.634311512415351</v>
       </c>
       <c r="J14" s="42"/>
       <c r="K14" s="43"/>
@@ -4401,15 +4410,15 @@
       <c r="E17" s="8"/>
       <c r="F17" s="1">
         <f>Assignment10!G17</f>
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="G17" s="1">
         <f>E17+F17</f>
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="H17" s="2">
         <f t="shared" ref="H17:H22" si="2">IF($G$23&lt;&gt;0,G17/$G$23,"-")</f>
-        <v>0.11700468018720749</v>
+        <v>9.5936794582392779E-2</v>
       </c>
       <c r="J17" s="49" t="s">
         <v>48</v>
@@ -4433,15 +4442,15 @@
       <c r="E18" s="8"/>
       <c r="F18" s="1">
         <f>Assignment10!G18</f>
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="G18" s="1">
         <f t="shared" ref="G18:G22" si="3">E18+F18</f>
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="H18" s="2">
         <f t="shared" si="2"/>
-        <v>8.2683307332293288E-2</v>
+        <v>6.5462753950338598E-2</v>
       </c>
       <c r="J18" s="50"/>
       <c r="K18" s="50"/>
@@ -4463,15 +4472,15 @@
       <c r="E19" s="8"/>
       <c r="F19" s="1">
         <f>Assignment10!G19</f>
-        <v>285</v>
+        <v>435</v>
       </c>
       <c r="G19" s="1">
         <f t="shared" si="3"/>
-        <v>285</v>
+        <v>435</v>
       </c>
       <c r="H19" s="2">
         <f t="shared" si="2"/>
-        <v>0.44461778471138846</v>
+        <v>0.49097065462753953</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -4484,15 +4493,15 @@
       <c r="E20" s="8"/>
       <c r="F20" s="1">
         <f>Assignment10!G20</f>
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="G20" s="1">
         <f t="shared" si="3"/>
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="H20" s="2">
         <f t="shared" si="2"/>
-        <v>0.10920436817472699</v>
+        <v>0.12415349887133183</v>
       </c>
       <c r="J20" s="51" t="s">
         <v>43</v>
@@ -4516,15 +4525,15 @@
       <c r="E21" s="8"/>
       <c r="F21" s="1">
         <f>Assignment10!G21</f>
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="G21" s="1">
         <f t="shared" si="3"/>
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="H21" s="2">
         <f t="shared" si="2"/>
-        <v>0.1482059282371295</v>
+        <v>0.14108352144469527</v>
       </c>
       <c r="J21" s="54"/>
       <c r="K21" s="55"/>
@@ -4546,15 +4555,15 @@
       <c r="E22" s="8"/>
       <c r="F22" s="1">
         <f>Assignment10!G22</f>
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="G22" s="1">
         <f t="shared" si="3"/>
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="H22" s="2">
         <f t="shared" si="2"/>
-        <v>9.8283931357254287E-2</v>
+        <v>8.2392776523702027E-2</v>
       </c>
       <c r="J22" s="54"/>
       <c r="K22" s="55"/>
@@ -4582,11 +4591,11 @@
       </c>
       <c r="F23" s="1">
         <f>SUM(F17:F22)</f>
-        <v>641</v>
+        <v>886</v>
       </c>
       <c r="G23" s="1">
         <f>SUM(G17:G22)</f>
-        <v>641</v>
+        <v>886</v>
       </c>
       <c r="H23" s="2">
         <f>SUM(H17:H22)</f>
@@ -4657,7 +4666,7 @@
       </c>
       <c r="H26" s="2">
         <f t="shared" ref="H26:H31" si="6">IF($G$32&lt;&gt;0,G26/$G$32,"-")</f>
-        <v>5.2631578947368418E-2</v>
+        <v>0.04</v>
       </c>
       <c r="J26" s="54"/>
       <c r="K26" s="55"/>
@@ -4686,7 +4695,7 @@
       </c>
       <c r="H27" s="2">
         <f t="shared" si="6"/>
-        <v>0.10526315789473684</v>
+        <v>0.08</v>
       </c>
       <c r="J27" s="54"/>
       <c r="K27" s="55"/>
@@ -4715,7 +4724,7 @@
       </c>
       <c r="H28" s="2">
         <f t="shared" si="6"/>
-        <v>0.42105263157894735</v>
+        <v>0.32</v>
       </c>
       <c r="J28" s="57"/>
       <c r="K28" s="58"/>
@@ -4744,7 +4753,7 @@
       </c>
       <c r="H29" s="2">
         <f t="shared" si="6"/>
-        <v>0.15789473684210525</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4756,15 +4765,15 @@
       <c r="E30" s="8"/>
       <c r="F30" s="1">
         <f>Assignment10!G30</f>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="G30" s="1">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="H30" s="2">
         <f t="shared" si="6"/>
-        <v>0.26315789473684209</v>
+        <v>0.44</v>
       </c>
       <c r="J30" s="20" t="s">
         <v>46</v>
@@ -4811,11 +4820,11 @@
       </c>
       <c r="F32" s="1">
         <f>SUM(F26:F31)</f>
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="G32" s="1">
         <f>SUM(G26:G31)</f>
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="H32" s="2">
         <f>SUM(H26:H31)</f>
@@ -4893,7 +4902,7 @@
       </c>
       <c r="H35" s="2">
         <f t="shared" ref="H35:H40" si="9">IF($G$41&lt;&gt;0,G35/$G$41,"-")</f>
-        <v>5.2631578947368418E-2</v>
+        <v>0.04</v>
       </c>
       <c r="J35" s="64"/>
       <c r="K35" s="65"/>
@@ -4922,7 +4931,7 @@
       </c>
       <c r="H36" s="2">
         <f t="shared" si="9"/>
-        <v>0.10526315789473684</v>
+        <v>0.08</v>
       </c>
       <c r="J36" s="64"/>
       <c r="K36" s="65"/>
@@ -4951,7 +4960,7 @@
       </c>
       <c r="H37" s="2">
         <f t="shared" si="9"/>
-        <v>0.42105263157894735</v>
+        <v>0.32</v>
       </c>
       <c r="J37" s="64"/>
       <c r="K37" s="65"/>
@@ -4980,7 +4989,7 @@
       </c>
       <c r="H38" s="2">
         <f t="shared" si="9"/>
-        <v>0.15789473684210525</v>
+        <v>0.12</v>
       </c>
       <c r="J38" s="64"/>
       <c r="K38" s="65"/>
@@ -5001,15 +5010,15 @@
       <c r="E39" s="8"/>
       <c r="F39" s="1">
         <f>Assignment10!G39</f>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="G39" s="1">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="H39" s="2">
         <f t="shared" si="9"/>
-        <v>0.26315789473684209</v>
+        <v>0.44</v>
       </c>
       <c r="J39" s="64"/>
       <c r="K39" s="65"/>
@@ -5062,11 +5071,11 @@
       </c>
       <c r="F41" s="1">
         <f>SUM(F35:F40)</f>
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="G41" s="1">
         <f>SUM(G35:G40)</f>
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="H41" s="2">
         <f>SUM(H35:H40)</f>
@@ -5375,12 +5384,12 @@
       </c>
       <c r="F7" s="1">
         <f>Assignment11!H7</f>
-        <v>0</v>
+        <v>316</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="1">
         <f t="shared" ref="H7:H10" si="0">E7+F7</f>
-        <v>0</v>
+        <v>316</v>
       </c>
       <c r="J7" s="33" t="s">
         <v>37</v>
@@ -5408,12 +5417,12 @@
       </c>
       <c r="F8" s="1">
         <f>Assignment11!H8</f>
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="J8" s="36"/>
       <c r="K8" s="37"/>
@@ -5473,12 +5482,12 @@
       </c>
       <c r="F10" s="1">
         <f>Assignment11!H10</f>
-        <v>1059</v>
+        <v>1235</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="1">
         <f t="shared" si="0"/>
-        <v>1059</v>
+        <v>1235</v>
       </c>
       <c r="J10" s="36"/>
       <c r="K10" s="37"/>
@@ -5538,12 +5547,12 @@
       </c>
       <c r="F12" s="1">
         <f>Assignment11!H12</f>
-        <v>1059</v>
+        <v>1235</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="1">
         <f t="shared" ref="H12:H13" si="1">E12+F12</f>
-        <v>1059</v>
+        <v>1235</v>
       </c>
       <c r="J12" s="36"/>
       <c r="K12" s="37"/>
@@ -5569,12 +5578,12 @@
       </c>
       <c r="F13" s="1">
         <f>Assignment11!H13</f>
-        <v>1085</v>
+        <v>1437</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="1">
         <f t="shared" si="1"/>
-        <v>1085</v>
+        <v>1437</v>
       </c>
       <c r="J13" s="33" t="s">
         <v>40</v>
@@ -5605,7 +5614,7 @@
       <c r="G14" s="3"/>
       <c r="H14" s="1">
         <f>IF($G$23&lt;&gt;0,60*H12/$G$23,"-")</f>
-        <v>99.126365054602189</v>
+        <v>83.634311512415351</v>
       </c>
       <c r="J14" s="42"/>
       <c r="K14" s="43"/>
@@ -5676,15 +5685,15 @@
       <c r="E17" s="8"/>
       <c r="F17" s="1">
         <f>Assignment11!G17</f>
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="G17" s="1">
         <f>E17+F17</f>
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="H17" s="2">
         <f t="shared" ref="H17:H22" si="2">IF($G$23&lt;&gt;0,G17/$G$23,"-")</f>
-        <v>0.11700468018720749</v>
+        <v>9.5936794582392779E-2</v>
       </c>
       <c r="J17" s="49" t="s">
         <v>48</v>
@@ -5708,15 +5717,15 @@
       <c r="E18" s="8"/>
       <c r="F18" s="1">
         <f>Assignment11!G18</f>
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="G18" s="1">
         <f t="shared" ref="G18:G22" si="3">E18+F18</f>
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="H18" s="2">
         <f t="shared" si="2"/>
-        <v>8.2683307332293288E-2</v>
+        <v>6.5462753950338598E-2</v>
       </c>
       <c r="J18" s="50"/>
       <c r="K18" s="50"/>
@@ -5738,15 +5747,15 @@
       <c r="E19" s="8"/>
       <c r="F19" s="1">
         <f>Assignment11!G19</f>
-        <v>285</v>
+        <v>435</v>
       </c>
       <c r="G19" s="1">
         <f t="shared" si="3"/>
-        <v>285</v>
+        <v>435</v>
       </c>
       <c r="H19" s="2">
         <f t="shared" si="2"/>
-        <v>0.44461778471138846</v>
+        <v>0.49097065462753953</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -5759,15 +5768,15 @@
       <c r="E20" s="8"/>
       <c r="F20" s="1">
         <f>Assignment11!G20</f>
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="G20" s="1">
         <f t="shared" si="3"/>
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="H20" s="2">
         <f t="shared" si="2"/>
-        <v>0.10920436817472699</v>
+        <v>0.12415349887133183</v>
       </c>
       <c r="J20" s="51" t="s">
         <v>43</v>
@@ -5791,15 +5800,15 @@
       <c r="E21" s="8"/>
       <c r="F21" s="1">
         <f>Assignment11!G21</f>
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="G21" s="1">
         <f t="shared" si="3"/>
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="H21" s="2">
         <f t="shared" si="2"/>
-        <v>0.1482059282371295</v>
+        <v>0.14108352144469527</v>
       </c>
       <c r="J21" s="54"/>
       <c r="K21" s="55"/>
@@ -5821,15 +5830,15 @@
       <c r="E22" s="8"/>
       <c r="F22" s="1">
         <f>Assignment11!G22</f>
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="G22" s="1">
         <f t="shared" si="3"/>
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="H22" s="2">
         <f t="shared" si="2"/>
-        <v>9.8283931357254287E-2</v>
+        <v>8.2392776523702027E-2</v>
       </c>
       <c r="J22" s="54"/>
       <c r="K22" s="55"/>
@@ -5857,11 +5866,11 @@
       </c>
       <c r="F23" s="1">
         <f>SUM(F17:F22)</f>
-        <v>641</v>
+        <v>886</v>
       </c>
       <c r="G23" s="1">
         <f>SUM(G17:G22)</f>
-        <v>641</v>
+        <v>886</v>
       </c>
       <c r="H23" s="2">
         <f>SUM(H17:H22)</f>
@@ -5932,7 +5941,7 @@
       </c>
       <c r="H26" s="2">
         <f t="shared" ref="H26:H31" si="6">IF($G$32&lt;&gt;0,G26/$G$32,"-")</f>
-        <v>5.2631578947368418E-2</v>
+        <v>0.04</v>
       </c>
       <c r="J26" s="54"/>
       <c r="K26" s="55"/>
@@ -5961,7 +5970,7 @@
       </c>
       <c r="H27" s="2">
         <f t="shared" si="6"/>
-        <v>0.10526315789473684</v>
+        <v>0.08</v>
       </c>
       <c r="J27" s="54"/>
       <c r="K27" s="55"/>
@@ -5990,7 +5999,7 @@
       </c>
       <c r="H28" s="2">
         <f t="shared" si="6"/>
-        <v>0.42105263157894735</v>
+        <v>0.32</v>
       </c>
       <c r="J28" s="57"/>
       <c r="K28" s="58"/>
@@ -6019,7 +6028,7 @@
       </c>
       <c r="H29" s="2">
         <f t="shared" si="6"/>
-        <v>0.15789473684210525</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6031,15 +6040,15 @@
       <c r="E30" s="8"/>
       <c r="F30" s="1">
         <f>Assignment11!G30</f>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="G30" s="1">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="H30" s="2">
         <f t="shared" si="6"/>
-        <v>0.26315789473684209</v>
+        <v>0.44</v>
       </c>
       <c r="J30" s="20" t="s">
         <v>46</v>
@@ -6086,11 +6095,11 @@
       </c>
       <c r="F32" s="1">
         <f>SUM(F26:F31)</f>
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="G32" s="1">
         <f>SUM(G26:G31)</f>
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="H32" s="2">
         <f>SUM(H26:H31)</f>
@@ -6168,7 +6177,7 @@
       </c>
       <c r="H35" s="2">
         <f t="shared" ref="H35:H40" si="9">IF($G$41&lt;&gt;0,G35/$G$41,"-")</f>
-        <v>5.2631578947368418E-2</v>
+        <v>0.04</v>
       </c>
       <c r="J35" s="64"/>
       <c r="K35" s="65"/>
@@ -6197,7 +6206,7 @@
       </c>
       <c r="H36" s="2">
         <f t="shared" si="9"/>
-        <v>0.10526315789473684</v>
+        <v>0.08</v>
       </c>
       <c r="J36" s="64"/>
       <c r="K36" s="65"/>
@@ -6226,7 +6235,7 @@
       </c>
       <c r="H37" s="2">
         <f t="shared" si="9"/>
-        <v>0.42105263157894735</v>
+        <v>0.32</v>
       </c>
       <c r="J37" s="64"/>
       <c r="K37" s="65"/>
@@ -6255,7 +6264,7 @@
       </c>
       <c r="H38" s="2">
         <f t="shared" si="9"/>
-        <v>0.15789473684210525</v>
+        <v>0.12</v>
       </c>
       <c r="J38" s="64"/>
       <c r="K38" s="65"/>
@@ -6276,15 +6285,15 @@
       <c r="E39" s="8"/>
       <c r="F39" s="1">
         <f>Assignment11!G39</f>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="G39" s="1">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="H39" s="2">
         <f t="shared" si="9"/>
-        <v>0.26315789473684209</v>
+        <v>0.44</v>
       </c>
       <c r="J39" s="64"/>
       <c r="K39" s="65"/>
@@ -6337,11 +6346,11 @@
       </c>
       <c r="F41" s="1">
         <f>SUM(F35:F40)</f>
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="G41" s="1">
         <f>SUM(G35:G40)</f>
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="H41" s="2">
         <f>SUM(H35:H40)</f>
@@ -7818,7 +7827,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T47"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="J31" sqref="J31:R42"/>
     </sheetView>
   </sheetViews>
@@ -9138,7 +9147,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="J31" sqref="J31:R42"/>
     </sheetView>
   </sheetViews>
@@ -10473,7 +10482,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T47"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J31" sqref="J31:R42"/>
     </sheetView>
   </sheetViews>
@@ -11811,7 +11820,7 @@
   <dimension ref="A1:T47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D2"/>
+      <selection activeCell="J31" sqref="J31:R42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11850,7 +11859,9 @@
       <c r="E2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="23"/>
+      <c r="F2" s="23">
+        <v>42500</v>
+      </c>
       <c r="G2" s="22"/>
       <c r="H2" s="22"/>
       <c r="J2" s="13" t="s">
@@ -11871,13 +11882,17 @@
       <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="22"/>
+      <c r="B3" s="22" t="s">
+        <v>67</v>
+      </c>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
       <c r="E3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="22"/>
+      <c r="F3" s="22" t="s">
+        <v>68</v>
+      </c>
       <c r="G3" s="22"/>
       <c r="H3" s="22"/>
       <c r="J3" s="13" t="s">
@@ -11896,13 +11911,17 @@
       <c r="A4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="22"/>
+      <c r="B4" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="C4" s="22"/>
       <c r="D4" s="22"/>
       <c r="E4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="22"/>
+      <c r="F4" s="22" t="s">
+        <v>56</v>
+      </c>
       <c r="G4" s="22"/>
       <c r="H4" s="22"/>
       <c r="J4" s="24" t="s">
@@ -11957,7 +11976,7 @@
         <v>15</v>
       </c>
       <c r="E7" s="7">
-        <v>0</v>
+        <v>316</v>
       </c>
       <c r="F7" s="1">
         <f>Assignment5!H7</f>
@@ -11966,7 +11985,7 @@
       <c r="G7" s="3"/>
       <c r="H7" s="1">
         <f t="shared" ref="H7:H10" si="0">E7+F7</f>
-        <v>0</v>
+        <v>316</v>
       </c>
       <c r="J7" s="33" t="s">
         <v>37</v>
@@ -11990,7 +12009,7 @@
         <v>15</v>
       </c>
       <c r="E8" s="7">
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="F8" s="1">
         <f>Assignment5!H8</f>
@@ -11999,7 +12018,7 @@
       <c r="G8" s="3"/>
       <c r="H8" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="J8" s="36"/>
       <c r="K8" s="37"/>
@@ -12055,7 +12074,7 @@
       </c>
       <c r="E10" s="1">
         <f>E13-E7+E8-E11</f>
-        <v>0</v>
+        <v>176</v>
       </c>
       <c r="F10" s="1">
         <f>Assignment5!H10</f>
@@ -12064,7 +12083,7 @@
       <c r="G10" s="3"/>
       <c r="H10" s="1">
         <f t="shared" si="0"/>
-        <v>1059</v>
+        <v>1235</v>
       </c>
       <c r="J10" s="36"/>
       <c r="K10" s="37"/>
@@ -12120,7 +12139,7 @@
       </c>
       <c r="E12" s="1">
         <f>E10+E9</f>
-        <v>0</v>
+        <v>176</v>
       </c>
       <c r="F12" s="1">
         <f>Assignment5!H12</f>
@@ -12129,7 +12148,7 @@
       <c r="G12" s="3"/>
       <c r="H12" s="1">
         <f t="shared" ref="H12:H13" si="1">E12+F12</f>
-        <v>1059</v>
+        <v>1235</v>
       </c>
       <c r="J12" s="36"/>
       <c r="K12" s="37"/>
@@ -12151,7 +12170,7 @@
         <v>15</v>
       </c>
       <c r="E13" s="7">
-        <v>0</v>
+        <v>352</v>
       </c>
       <c r="F13" s="1">
         <f>Assignment5!H13</f>
@@ -12160,7 +12179,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="1">
         <f t="shared" si="1"/>
-        <v>1085</v>
+        <v>1437</v>
       </c>
       <c r="J13" s="33" t="s">
         <v>40</v>
@@ -12180,18 +12199,18 @@
       <c r="C14" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="E14" s="1" t="str">
+      <c r="E14" s="1">
         <f>IF($E$23&lt;&gt;0,60*E12/$E$23,"-")</f>
-        <v>-</v>
-      </c>
-      <c r="F14" s="1" t="str">
+        <v>43.102040816326529</v>
+      </c>
+      <c r="F14" s="1">
         <f>IF($E$23&lt;&gt;0,60*F12/$E$23,"-")</f>
-        <v>-</v>
+        <v>259.34693877551018</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="1">
         <f>IF($G$23&lt;&gt;0,60*H12/$G$23,"-")</f>
-        <v>99.126365054602189</v>
+        <v>83.634311512415351</v>
       </c>
       <c r="J14" s="42"/>
       <c r="K14" s="43"/>
@@ -12258,19 +12277,23 @@
       </c>
       <c r="B17" s="29"/>
       <c r="C17" s="29"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+      <c r="D17" s="8">
+        <v>10</v>
+      </c>
+      <c r="E17" s="8">
+        <v>10</v>
+      </c>
       <c r="F17" s="1">
         <f>Assignment5!G17</f>
         <v>75</v>
       </c>
       <c r="G17" s="1">
         <f>E17+F17</f>
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="H17" s="2">
         <f t="shared" ref="H17:H22" si="2">IF($G$23&lt;&gt;0,G17/$G$23,"-")</f>
-        <v>0.11700468018720749</v>
+        <v>9.5936794582392779E-2</v>
       </c>
       <c r="J17" s="49" t="s">
         <v>48</v>
@@ -12290,19 +12313,23 @@
       </c>
       <c r="B18" s="29"/>
       <c r="C18" s="29"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
+      <c r="D18" s="8">
+        <v>10</v>
+      </c>
+      <c r="E18" s="8">
+        <v>5</v>
+      </c>
       <c r="F18" s="1">
         <f>Assignment5!G18</f>
         <v>53</v>
       </c>
       <c r="G18" s="1">
         <f t="shared" ref="G18:G22" si="3">E18+F18</f>
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="H18" s="2">
         <f t="shared" si="2"/>
-        <v>8.2683307332293288E-2</v>
+        <v>6.5462753950338598E-2</v>
       </c>
       <c r="J18" s="50"/>
       <c r="K18" s="50"/>
@@ -12320,19 +12347,23 @@
       </c>
       <c r="B19" s="29"/>
       <c r="C19" s="29"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
+      <c r="D19" s="8">
+        <v>60</v>
+      </c>
+      <c r="E19" s="8">
+        <v>150</v>
+      </c>
       <c r="F19" s="1">
         <f>Assignment5!G19</f>
         <v>285</v>
       </c>
       <c r="G19" s="1">
         <f t="shared" si="3"/>
-        <v>285</v>
+        <v>435</v>
       </c>
       <c r="H19" s="2">
         <f t="shared" si="2"/>
-        <v>0.44461778471138846</v>
+        <v>0.49097065462753953</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -12341,19 +12372,23 @@
       </c>
       <c r="B20" s="29"/>
       <c r="C20" s="29"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
+      <c r="D20" s="8">
+        <v>30</v>
+      </c>
+      <c r="E20" s="8">
+        <v>40</v>
+      </c>
       <c r="F20" s="1">
         <f>Assignment5!G20</f>
         <v>70</v>
       </c>
       <c r="G20" s="1">
         <f t="shared" si="3"/>
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="H20" s="2">
         <f t="shared" si="2"/>
-        <v>0.10920436817472699</v>
+        <v>0.12415349887133183</v>
       </c>
       <c r="J20" s="51" t="s">
         <v>43</v>
@@ -12373,19 +12408,23 @@
       </c>
       <c r="B21" s="29"/>
       <c r="C21" s="29"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
+      <c r="D21" s="8">
+        <v>30</v>
+      </c>
+      <c r="E21" s="8">
+        <v>30</v>
+      </c>
       <c r="F21" s="1">
         <f>Assignment5!G21</f>
         <v>95</v>
       </c>
       <c r="G21" s="1">
         <f t="shared" si="3"/>
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="H21" s="2">
         <f t="shared" si="2"/>
-        <v>0.1482059282371295</v>
+        <v>0.14108352144469527</v>
       </c>
       <c r="J21" s="54"/>
       <c r="K21" s="55"/>
@@ -12403,19 +12442,23 @@
       </c>
       <c r="B22" s="29"/>
       <c r="C22" s="29"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
+      <c r="D22" s="8">
+        <v>10</v>
+      </c>
+      <c r="E22" s="8">
+        <v>10</v>
+      </c>
       <c r="F22" s="1">
         <f>Assignment5!G22</f>
         <v>63</v>
       </c>
       <c r="G22" s="1">
         <f t="shared" si="3"/>
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="H22" s="2">
         <f t="shared" si="2"/>
-        <v>9.8283931357254287E-2</v>
+        <v>8.2392776523702027E-2</v>
       </c>
       <c r="J22" s="54"/>
       <c r="K22" s="55"/>
@@ -12435,11 +12478,11 @@
       <c r="C23" s="29"/>
       <c r="D23" s="1">
         <f t="shared" ref="D23:E23" si="4">SUM(D17:D22)</f>
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="E23" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>245</v>
       </c>
       <c r="F23" s="1">
         <f>SUM(F17:F22)</f>
@@ -12447,7 +12490,7 @@
       </c>
       <c r="G23" s="1">
         <f>SUM(G17:G22)</f>
-        <v>641</v>
+        <v>886</v>
       </c>
       <c r="H23" s="2">
         <f>SUM(H17:H22)</f>
@@ -12507,7 +12550,9 @@
       </c>
       <c r="B26" s="29"/>
       <c r="C26" s="29"/>
-      <c r="E26" s="8"/>
+      <c r="E26" s="8">
+        <v>0</v>
+      </c>
       <c r="F26" s="1">
         <f>Assignment5!G26</f>
         <v>1</v>
@@ -12518,7 +12563,7 @@
       </c>
       <c r="H26" s="2">
         <f t="shared" ref="H26:H31" si="6">IF($G$32&lt;&gt;0,G26/$G$32,"-")</f>
-        <v>5.2631578947368418E-2</v>
+        <v>0.04</v>
       </c>
       <c r="J26" s="54"/>
       <c r="K26" s="55"/>
@@ -12536,7 +12581,9 @@
       </c>
       <c r="B27" s="29"/>
       <c r="C27" s="29"/>
-      <c r="E27" s="8"/>
+      <c r="E27" s="8">
+        <v>0</v>
+      </c>
       <c r="F27" s="1">
         <f>Assignment5!G27</f>
         <v>2</v>
@@ -12547,7 +12594,7 @@
       </c>
       <c r="H27" s="2">
         <f t="shared" si="6"/>
-        <v>0.10526315789473684</v>
+        <v>0.08</v>
       </c>
       <c r="J27" s="54"/>
       <c r="K27" s="55"/>
@@ -12565,7 +12612,9 @@
       </c>
       <c r="B28" s="29"/>
       <c r="C28" s="29"/>
-      <c r="E28" s="8"/>
+      <c r="E28" s="8">
+        <v>0</v>
+      </c>
       <c r="F28" s="1">
         <f>Assignment5!G28</f>
         <v>8</v>
@@ -12576,7 +12625,7 @@
       </c>
       <c r="H28" s="2">
         <f t="shared" si="6"/>
-        <v>0.42105263157894735</v>
+        <v>0.32</v>
       </c>
       <c r="J28" s="57"/>
       <c r="K28" s="58"/>
@@ -12594,7 +12643,9 @@
       </c>
       <c r="B29" s="29"/>
       <c r="C29" s="29"/>
-      <c r="E29" s="8"/>
+      <c r="E29" s="8">
+        <v>0</v>
+      </c>
       <c r="F29" s="1">
         <f>Assignment5!G29</f>
         <v>3</v>
@@ -12605,7 +12656,7 @@
       </c>
       <c r="H29" s="2">
         <f t="shared" si="6"/>
-        <v>0.15789473684210525</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -12614,18 +12665,20 @@
       </c>
       <c r="B30" s="29"/>
       <c r="C30" s="29"/>
-      <c r="E30" s="8"/>
+      <c r="E30" s="8">
+        <v>6</v>
+      </c>
       <c r="F30" s="1">
         <f>Assignment5!G30</f>
         <v>5</v>
       </c>
       <c r="G30" s="1">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="H30" s="2">
         <f t="shared" si="6"/>
-        <v>0.26315789473684209</v>
+        <v>0.44</v>
       </c>
       <c r="J30" s="20" t="s">
         <v>46</v>
@@ -12637,7 +12690,9 @@
       </c>
       <c r="B31" s="29"/>
       <c r="C31" s="29"/>
-      <c r="E31" s="8"/>
+      <c r="E31" s="8">
+        <v>0</v>
+      </c>
       <c r="F31" s="1">
         <f>Assignment5!G31</f>
         <v>0</v>
@@ -12650,7 +12705,9 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="J31" s="61"/>
+      <c r="J31" s="61" t="s">
+        <v>69</v>
+      </c>
       <c r="K31" s="62"/>
       <c r="L31" s="62"/>
       <c r="M31" s="62"/>
@@ -12668,7 +12725,7 @@
       <c r="C32" s="29"/>
       <c r="E32" s="1">
         <f t="shared" ref="E32" si="7">SUM(E26:E31)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F32" s="1">
         <f>SUM(F26:F31)</f>
@@ -12676,7 +12733,7 @@
       </c>
       <c r="G32" s="1">
         <f>SUM(G26:G31)</f>
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="H32" s="2">
         <f>SUM(H26:H31)</f>
@@ -12743,7 +12800,9 @@
       </c>
       <c r="B35" s="29"/>
       <c r="C35" s="29"/>
-      <c r="E35" s="8"/>
+      <c r="E35" s="8">
+        <v>0</v>
+      </c>
       <c r="F35" s="1">
         <f>Assignment5!G35</f>
         <v>1</v>
@@ -12754,7 +12813,7 @@
       </c>
       <c r="H35" s="2">
         <f t="shared" ref="H35:H40" si="9">IF($G$41&lt;&gt;0,G35/$G$41,"-")</f>
-        <v>5.2631578947368418E-2</v>
+        <v>0.04</v>
       </c>
       <c r="J35" s="64"/>
       <c r="K35" s="65"/>
@@ -12772,7 +12831,9 @@
       </c>
       <c r="B36" s="29"/>
       <c r="C36" s="29"/>
-      <c r="E36" s="8"/>
+      <c r="E36" s="8">
+        <v>0</v>
+      </c>
       <c r="F36" s="1">
         <f>Assignment5!G36</f>
         <v>2</v>
@@ -12783,7 +12844,7 @@
       </c>
       <c r="H36" s="2">
         <f t="shared" si="9"/>
-        <v>0.10526315789473684</v>
+        <v>0.08</v>
       </c>
       <c r="J36" s="64"/>
       <c r="K36" s="65"/>
@@ -12801,7 +12862,9 @@
       </c>
       <c r="B37" s="29"/>
       <c r="C37" s="29"/>
-      <c r="E37" s="8"/>
+      <c r="E37" s="8">
+        <v>0</v>
+      </c>
       <c r="F37" s="1">
         <f>Assignment5!G37</f>
         <v>8</v>
@@ -12812,7 +12875,7 @@
       </c>
       <c r="H37" s="2">
         <f t="shared" si="9"/>
-        <v>0.42105263157894735</v>
+        <v>0.32</v>
       </c>
       <c r="J37" s="64"/>
       <c r="K37" s="65"/>
@@ -12830,7 +12893,9 @@
       </c>
       <c r="B38" s="29"/>
       <c r="C38" s="29"/>
-      <c r="E38" s="8"/>
+      <c r="E38" s="8">
+        <v>0</v>
+      </c>
       <c r="F38" s="1">
         <f>Assignment5!G38</f>
         <v>3</v>
@@ -12841,7 +12906,7 @@
       </c>
       <c r="H38" s="2">
         <f t="shared" si="9"/>
-        <v>0.15789473684210525</v>
+        <v>0.12</v>
       </c>
       <c r="J38" s="64"/>
       <c r="K38" s="65"/>
@@ -12859,18 +12924,20 @@
       </c>
       <c r="B39" s="29"/>
       <c r="C39" s="29"/>
-      <c r="E39" s="8"/>
+      <c r="E39" s="8">
+        <v>6</v>
+      </c>
       <c r="F39" s="1">
         <f>Assignment5!G39</f>
         <v>5</v>
       </c>
       <c r="G39" s="1">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="H39" s="2">
         <f t="shared" si="9"/>
-        <v>0.26315789473684209</v>
+        <v>0.44</v>
       </c>
       <c r="J39" s="64"/>
       <c r="K39" s="65"/>
@@ -12888,7 +12955,9 @@
       </c>
       <c r="B40" s="29"/>
       <c r="C40" s="29"/>
-      <c r="E40" s="8"/>
+      <c r="E40" s="8">
+        <v>0</v>
+      </c>
       <c r="F40" s="1">
         <f>Assignment5!G40</f>
         <v>0</v>
@@ -12919,7 +12988,7 @@
       <c r="C41" s="29"/>
       <c r="E41" s="1">
         <f t="shared" ref="E41" si="10">SUM(E35:E40)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F41" s="1">
         <f>SUM(F35:F40)</f>
@@ -12927,7 +12996,7 @@
       </c>
       <c r="G41" s="1">
         <f>SUM(G35:G40)</f>
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="H41" s="2">
         <f>SUM(H35:H40)</f>
@@ -12974,7 +13043,9 @@
     </row>
     <row r="43" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="44" spans="1:18" ht="14.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J44" s="70"/>
+      <c r="J44" s="70" t="s">
+        <v>52</v>
+      </c>
       <c r="K44" s="71"/>
       <c r="L44" s="72"/>
       <c r="M44" s="73" t="s">
@@ -13233,12 +13304,12 @@
       </c>
       <c r="F7" s="1">
         <f>Assignment6!H7</f>
-        <v>0</v>
+        <v>316</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="1">
         <f t="shared" ref="H7:H10" si="0">E7+F7</f>
-        <v>0</v>
+        <v>316</v>
       </c>
       <c r="J7" s="33" t="s">
         <v>37</v>
@@ -13266,12 +13337,12 @@
       </c>
       <c r="F8" s="1">
         <f>Assignment6!H8</f>
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="J8" s="36"/>
       <c r="K8" s="37"/>
@@ -13331,12 +13402,12 @@
       </c>
       <c r="F10" s="1">
         <f>Assignment6!H10</f>
-        <v>1059</v>
+        <v>1235</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="1">
         <f t="shared" si="0"/>
-        <v>1059</v>
+        <v>1235</v>
       </c>
       <c r="J10" s="36"/>
       <c r="K10" s="37"/>
@@ -13396,12 +13467,12 @@
       </c>
       <c r="F12" s="1">
         <f>Assignment6!H12</f>
-        <v>1059</v>
+        <v>1235</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="1">
         <f t="shared" ref="H12:H13" si="1">E12+F12</f>
-        <v>1059</v>
+        <v>1235</v>
       </c>
       <c r="J12" s="36"/>
       <c r="K12" s="37"/>
@@ -13427,12 +13498,12 @@
       </c>
       <c r="F13" s="1">
         <f>Assignment6!H13</f>
-        <v>1085</v>
+        <v>1437</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="1">
         <f t="shared" si="1"/>
-        <v>1085</v>
+        <v>1437</v>
       </c>
       <c r="J13" s="33" t="s">
         <v>40</v>
@@ -13463,7 +13534,7 @@
       <c r="G14" s="3"/>
       <c r="H14" s="1">
         <f>IF($G$23&lt;&gt;0,60*H12/$G$23,"-")</f>
-        <v>99.126365054602189</v>
+        <v>83.634311512415351</v>
       </c>
       <c r="J14" s="42"/>
       <c r="K14" s="43"/>
@@ -13534,15 +13605,15 @@
       <c r="E17" s="8"/>
       <c r="F17" s="1">
         <f>Assignment6!G17</f>
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="G17" s="1">
         <f>E17+F17</f>
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="H17" s="2">
         <f t="shared" ref="H17:H22" si="2">IF($G$23&lt;&gt;0,G17/$G$23,"-")</f>
-        <v>0.11700468018720749</v>
+        <v>9.5936794582392779E-2</v>
       </c>
       <c r="J17" s="49" t="s">
         <v>48</v>
@@ -13566,15 +13637,15 @@
       <c r="E18" s="8"/>
       <c r="F18" s="1">
         <f>Assignment6!G18</f>
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="G18" s="1">
         <f t="shared" ref="G18:G22" si="3">E18+F18</f>
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="H18" s="2">
         <f t="shared" si="2"/>
-        <v>8.2683307332293288E-2</v>
+        <v>6.5462753950338598E-2</v>
       </c>
       <c r="J18" s="50"/>
       <c r="K18" s="50"/>
@@ -13596,15 +13667,15 @@
       <c r="E19" s="8"/>
       <c r="F19" s="1">
         <f>Assignment6!G19</f>
-        <v>285</v>
+        <v>435</v>
       </c>
       <c r="G19" s="1">
         <f t="shared" si="3"/>
-        <v>285</v>
+        <v>435</v>
       </c>
       <c r="H19" s="2">
         <f t="shared" si="2"/>
-        <v>0.44461778471138846</v>
+        <v>0.49097065462753953</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -13617,15 +13688,15 @@
       <c r="E20" s="8"/>
       <c r="F20" s="1">
         <f>Assignment6!G20</f>
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="G20" s="1">
         <f t="shared" si="3"/>
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="H20" s="2">
         <f t="shared" si="2"/>
-        <v>0.10920436817472699</v>
+        <v>0.12415349887133183</v>
       </c>
       <c r="J20" s="51" t="s">
         <v>43</v>
@@ -13649,15 +13720,15 @@
       <c r="E21" s="8"/>
       <c r="F21" s="1">
         <f>Assignment6!G21</f>
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="G21" s="1">
         <f t="shared" si="3"/>
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="H21" s="2">
         <f t="shared" si="2"/>
-        <v>0.1482059282371295</v>
+        <v>0.14108352144469527</v>
       </c>
       <c r="J21" s="54"/>
       <c r="K21" s="55"/>
@@ -13679,15 +13750,15 @@
       <c r="E22" s="8"/>
       <c r="F22" s="1">
         <f>Assignment6!G22</f>
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="G22" s="1">
         <f t="shared" si="3"/>
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="H22" s="2">
         <f t="shared" si="2"/>
-        <v>9.8283931357254287E-2</v>
+        <v>8.2392776523702027E-2</v>
       </c>
       <c r="J22" s="54"/>
       <c r="K22" s="55"/>
@@ -13715,11 +13786,11 @@
       </c>
       <c r="F23" s="1">
         <f>SUM(F17:F22)</f>
-        <v>641</v>
+        <v>886</v>
       </c>
       <c r="G23" s="1">
         <f>SUM(G17:G22)</f>
-        <v>641</v>
+        <v>886</v>
       </c>
       <c r="H23" s="2">
         <f>SUM(H17:H22)</f>
@@ -13790,7 +13861,7 @@
       </c>
       <c r="H26" s="2">
         <f t="shared" ref="H26:H31" si="6">IF($G$32&lt;&gt;0,G26/$G$32,"-")</f>
-        <v>5.2631578947368418E-2</v>
+        <v>0.04</v>
       </c>
       <c r="J26" s="54"/>
       <c r="K26" s="55"/>
@@ -13819,7 +13890,7 @@
       </c>
       <c r="H27" s="2">
         <f t="shared" si="6"/>
-        <v>0.10526315789473684</v>
+        <v>0.08</v>
       </c>
       <c r="J27" s="54"/>
       <c r="K27" s="55"/>
@@ -13848,7 +13919,7 @@
       </c>
       <c r="H28" s="2">
         <f t="shared" si="6"/>
-        <v>0.42105263157894735</v>
+        <v>0.32</v>
       </c>
       <c r="J28" s="57"/>
       <c r="K28" s="58"/>
@@ -13877,7 +13948,7 @@
       </c>
       <c r="H29" s="2">
         <f t="shared" si="6"/>
-        <v>0.15789473684210525</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -13889,15 +13960,15 @@
       <c r="E30" s="8"/>
       <c r="F30" s="1">
         <f>Assignment6!G30</f>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="G30" s="1">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="H30" s="2">
         <f t="shared" si="6"/>
-        <v>0.26315789473684209</v>
+        <v>0.44</v>
       </c>
       <c r="J30" s="20" t="s">
         <v>46</v>
@@ -13944,11 +14015,11 @@
       </c>
       <c r="F32" s="1">
         <f>SUM(F26:F31)</f>
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="G32" s="1">
         <f>SUM(G26:G31)</f>
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="H32" s="2">
         <f>SUM(H26:H31)</f>
@@ -14026,7 +14097,7 @@
       </c>
       <c r="H35" s="2">
         <f t="shared" ref="H35:H40" si="9">IF($G$41&lt;&gt;0,G35/$G$41,"-")</f>
-        <v>5.2631578947368418E-2</v>
+        <v>0.04</v>
       </c>
       <c r="J35" s="64"/>
       <c r="K35" s="65"/>
@@ -14055,7 +14126,7 @@
       </c>
       <c r="H36" s="2">
         <f t="shared" si="9"/>
-        <v>0.10526315789473684</v>
+        <v>0.08</v>
       </c>
       <c r="J36" s="64"/>
       <c r="K36" s="65"/>
@@ -14084,7 +14155,7 @@
       </c>
       <c r="H37" s="2">
         <f t="shared" si="9"/>
-        <v>0.42105263157894735</v>
+        <v>0.32</v>
       </c>
       <c r="J37" s="64"/>
       <c r="K37" s="65"/>
@@ -14113,7 +14184,7 @@
       </c>
       <c r="H38" s="2">
         <f t="shared" si="9"/>
-        <v>0.15789473684210525</v>
+        <v>0.12</v>
       </c>
       <c r="J38" s="64"/>
       <c r="K38" s="65"/>
@@ -14134,15 +14205,15 @@
       <c r="E39" s="8"/>
       <c r="F39" s="1">
         <f>Assignment6!G39</f>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="G39" s="1">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="H39" s="2">
         <f t="shared" si="9"/>
-        <v>0.26315789473684209</v>
+        <v>0.44</v>
       </c>
       <c r="J39" s="64"/>
       <c r="K39" s="65"/>
@@ -14195,11 +14266,11 @@
       </c>
       <c r="F41" s="1">
         <f>SUM(F35:F40)</f>
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="G41" s="1">
         <f>SUM(G35:G40)</f>
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="H41" s="2">
         <f>SUM(H35:H40)</f>
@@ -14505,12 +14576,12 @@
       </c>
       <c r="F7" s="1">
         <f>Assignment7!H7</f>
-        <v>0</v>
+        <v>316</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="1">
         <f t="shared" ref="H7:H10" si="0">E7+F7</f>
-        <v>0</v>
+        <v>316</v>
       </c>
       <c r="J7" s="33" t="s">
         <v>37</v>
@@ -14538,12 +14609,12 @@
       </c>
       <c r="F8" s="1">
         <f>Assignment7!H8</f>
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="J8" s="36"/>
       <c r="K8" s="37"/>
@@ -14603,12 +14674,12 @@
       </c>
       <c r="F10" s="1">
         <f>Assignment7!H10</f>
-        <v>1059</v>
+        <v>1235</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="1">
         <f t="shared" si="0"/>
-        <v>1059</v>
+        <v>1235</v>
       </c>
       <c r="J10" s="36"/>
       <c r="K10" s="37"/>
@@ -14668,12 +14739,12 @@
       </c>
       <c r="F12" s="1">
         <f>Assignment7!H12</f>
-        <v>1059</v>
+        <v>1235</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="1">
         <f t="shared" ref="H12:H13" si="1">E12+F12</f>
-        <v>1059</v>
+        <v>1235</v>
       </c>
       <c r="J12" s="36"/>
       <c r="K12" s="37"/>
@@ -14699,12 +14770,12 @@
       </c>
       <c r="F13" s="1">
         <f>Assignment7!H13</f>
-        <v>1085</v>
+        <v>1437</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="1">
         <f t="shared" si="1"/>
-        <v>1085</v>
+        <v>1437</v>
       </c>
       <c r="J13" s="33" t="s">
         <v>40</v>
@@ -14735,7 +14806,7 @@
       <c r="G14" s="3"/>
       <c r="H14" s="1">
         <f>IF($G$23&lt;&gt;0,60*H12/$G$23,"-")</f>
-        <v>99.126365054602189</v>
+        <v>83.634311512415351</v>
       </c>
       <c r="J14" s="42"/>
       <c r="K14" s="43"/>
@@ -14806,15 +14877,15 @@
       <c r="E17" s="8"/>
       <c r="F17" s="1">
         <f>Assignment7!G17</f>
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="G17" s="1">
         <f>E17+F17</f>
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="H17" s="2">
         <f t="shared" ref="H17:H22" si="2">IF($G$23&lt;&gt;0,G17/$G$23,"-")</f>
-        <v>0.11700468018720749</v>
+        <v>9.5936794582392779E-2</v>
       </c>
       <c r="J17" s="49" t="s">
         <v>48</v>
@@ -14838,15 +14909,15 @@
       <c r="E18" s="8"/>
       <c r="F18" s="1">
         <f>Assignment7!G18</f>
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="G18" s="1">
         <f t="shared" ref="G18:G22" si="3">E18+F18</f>
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="H18" s="2">
         <f t="shared" si="2"/>
-        <v>8.2683307332293288E-2</v>
+        <v>6.5462753950338598E-2</v>
       </c>
       <c r="J18" s="50"/>
       <c r="K18" s="50"/>
@@ -14868,15 +14939,15 @@
       <c r="E19" s="8"/>
       <c r="F19" s="1">
         <f>Assignment7!G19</f>
-        <v>285</v>
+        <v>435</v>
       </c>
       <c r="G19" s="1">
         <f t="shared" si="3"/>
-        <v>285</v>
+        <v>435</v>
       </c>
       <c r="H19" s="2">
         <f t="shared" si="2"/>
-        <v>0.44461778471138846</v>
+        <v>0.49097065462753953</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -14889,15 +14960,15 @@
       <c r="E20" s="8"/>
       <c r="F20" s="1">
         <f>Assignment7!G20</f>
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="G20" s="1">
         <f t="shared" si="3"/>
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="H20" s="2">
         <f t="shared" si="2"/>
-        <v>0.10920436817472699</v>
+        <v>0.12415349887133183</v>
       </c>
       <c r="J20" s="51" t="s">
         <v>43</v>
@@ -14921,15 +14992,15 @@
       <c r="E21" s="8"/>
       <c r="F21" s="1">
         <f>Assignment7!G21</f>
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="G21" s="1">
         <f t="shared" si="3"/>
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="H21" s="2">
         <f t="shared" si="2"/>
-        <v>0.1482059282371295</v>
+        <v>0.14108352144469527</v>
       </c>
       <c r="J21" s="54"/>
       <c r="K21" s="55"/>
@@ -14951,15 +15022,15 @@
       <c r="E22" s="8"/>
       <c r="F22" s="1">
         <f>Assignment7!G22</f>
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="G22" s="1">
         <f t="shared" si="3"/>
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="H22" s="2">
         <f t="shared" si="2"/>
-        <v>9.8283931357254287E-2</v>
+        <v>8.2392776523702027E-2</v>
       </c>
       <c r="J22" s="54"/>
       <c r="K22" s="55"/>
@@ -14987,11 +15058,11 @@
       </c>
       <c r="F23" s="1">
         <f>SUM(F17:F22)</f>
-        <v>641</v>
+        <v>886</v>
       </c>
       <c r="G23" s="1">
         <f>SUM(G17:G22)</f>
-        <v>641</v>
+        <v>886</v>
       </c>
       <c r="H23" s="2">
         <f>SUM(H17:H22)</f>
@@ -15062,7 +15133,7 @@
       </c>
       <c r="H26" s="2">
         <f t="shared" ref="H26:H31" si="6">IF($G$32&lt;&gt;0,G26/$G$32,"-")</f>
-        <v>5.2631578947368418E-2</v>
+        <v>0.04</v>
       </c>
       <c r="J26" s="54"/>
       <c r="K26" s="55"/>
@@ -15091,7 +15162,7 @@
       </c>
       <c r="H27" s="2">
         <f t="shared" si="6"/>
-        <v>0.10526315789473684</v>
+        <v>0.08</v>
       </c>
       <c r="J27" s="54"/>
       <c r="K27" s="55"/>
@@ -15120,7 +15191,7 @@
       </c>
       <c r="H28" s="2">
         <f t="shared" si="6"/>
-        <v>0.42105263157894735</v>
+        <v>0.32</v>
       </c>
       <c r="J28" s="57"/>
       <c r="K28" s="58"/>
@@ -15149,7 +15220,7 @@
       </c>
       <c r="H29" s="2">
         <f t="shared" si="6"/>
-        <v>0.15789473684210525</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -15161,15 +15232,15 @@
       <c r="E30" s="8"/>
       <c r="F30" s="1">
         <f>Assignment7!G30</f>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="G30" s="1">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="H30" s="2">
         <f t="shared" si="6"/>
-        <v>0.26315789473684209</v>
+        <v>0.44</v>
       </c>
       <c r="J30" s="20" t="s">
         <v>46</v>
@@ -15216,11 +15287,11 @@
       </c>
       <c r="F32" s="1">
         <f>SUM(F26:F31)</f>
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="G32" s="1">
         <f>SUM(G26:G31)</f>
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="H32" s="2">
         <f>SUM(H26:H31)</f>
@@ -15298,7 +15369,7 @@
       </c>
       <c r="H35" s="2">
         <f t="shared" ref="H35:H40" si="9">IF($G$41&lt;&gt;0,G35/$G$41,"-")</f>
-        <v>5.2631578947368418E-2</v>
+        <v>0.04</v>
       </c>
       <c r="J35" s="64"/>
       <c r="K35" s="65"/>
@@ -15327,7 +15398,7 @@
       </c>
       <c r="H36" s="2">
         <f t="shared" si="9"/>
-        <v>0.10526315789473684</v>
+        <v>0.08</v>
       </c>
       <c r="J36" s="64"/>
       <c r="K36" s="65"/>
@@ -15356,7 +15427,7 @@
       </c>
       <c r="H37" s="2">
         <f t="shared" si="9"/>
-        <v>0.42105263157894735</v>
+        <v>0.32</v>
       </c>
       <c r="J37" s="64"/>
       <c r="K37" s="65"/>
@@ -15385,7 +15456,7 @@
       </c>
       <c r="H38" s="2">
         <f t="shared" si="9"/>
-        <v>0.15789473684210525</v>
+        <v>0.12</v>
       </c>
       <c r="J38" s="64"/>
       <c r="K38" s="65"/>
@@ -15406,15 +15477,15 @@
       <c r="E39" s="8"/>
       <c r="F39" s="1">
         <f>Assignment7!G39</f>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="G39" s="1">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="H39" s="2">
         <f t="shared" si="9"/>
-        <v>0.26315789473684209</v>
+        <v>0.44</v>
       </c>
       <c r="J39" s="64"/>
       <c r="K39" s="65"/>
@@ -15467,11 +15538,11 @@
       </c>
       <c r="F41" s="1">
         <f>SUM(F35:F40)</f>
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="G41" s="1">
         <f>SUM(G35:G40)</f>
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="H41" s="2">
         <f>SUM(H35:H40)</f>
@@ -15781,12 +15852,12 @@
       </c>
       <c r="F7" s="1">
         <f>Assignment8!H7</f>
-        <v>0</v>
+        <v>316</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="1">
         <f t="shared" ref="H7:H10" si="0">E7+F7</f>
-        <v>0</v>
+        <v>316</v>
       </c>
       <c r="J7" s="33" t="s">
         <v>37</v>
@@ -15814,12 +15885,12 @@
       </c>
       <c r="F8" s="1">
         <f>Assignment8!H8</f>
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="J8" s="36"/>
       <c r="K8" s="37"/>
@@ -15879,12 +15950,12 @@
       </c>
       <c r="F10" s="1">
         <f>Assignment8!H10</f>
-        <v>1059</v>
+        <v>1235</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="1">
         <f t="shared" si="0"/>
-        <v>1059</v>
+        <v>1235</v>
       </c>
       <c r="J10" s="36"/>
       <c r="K10" s="37"/>
@@ -15944,12 +16015,12 @@
       </c>
       <c r="F12" s="1">
         <f>Assignment8!H12</f>
-        <v>1059</v>
+        <v>1235</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="1">
         <f t="shared" ref="H12:H13" si="1">E12+F12</f>
-        <v>1059</v>
+        <v>1235</v>
       </c>
       <c r="J12" s="36"/>
       <c r="K12" s="37"/>
@@ -15975,12 +16046,12 @@
       </c>
       <c r="F13" s="1">
         <f>Assignment8!H13</f>
-        <v>1085</v>
+        <v>1437</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="1">
         <f t="shared" si="1"/>
-        <v>1085</v>
+        <v>1437</v>
       </c>
       <c r="J13" s="33" t="s">
         <v>40</v>
@@ -16011,7 +16082,7 @@
       <c r="G14" s="3"/>
       <c r="H14" s="1">
         <f>IF($G$23&lt;&gt;0,60*H12/$G$23,"-")</f>
-        <v>99.126365054602189</v>
+        <v>83.634311512415351</v>
       </c>
       <c r="J14" s="42"/>
       <c r="K14" s="43"/>
@@ -16082,15 +16153,15 @@
       <c r="E17" s="8"/>
       <c r="F17" s="1">
         <f>Assignment8!G17</f>
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="G17" s="1">
         <f>E17+F17</f>
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="H17" s="2">
         <f t="shared" ref="H17:H22" si="2">IF($G$23&lt;&gt;0,G17/$G$23,"-")</f>
-        <v>0.11700468018720749</v>
+        <v>9.5936794582392779E-2</v>
       </c>
       <c r="J17" s="49" t="s">
         <v>48</v>
@@ -16114,15 +16185,15 @@
       <c r="E18" s="8"/>
       <c r="F18" s="1">
         <f>Assignment8!G18</f>
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="G18" s="1">
         <f t="shared" ref="G18:G22" si="3">E18+F18</f>
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="H18" s="2">
         <f t="shared" si="2"/>
-        <v>8.2683307332293288E-2</v>
+        <v>6.5462753950338598E-2</v>
       </c>
       <c r="J18" s="50"/>
       <c r="K18" s="50"/>
@@ -16144,15 +16215,15 @@
       <c r="E19" s="8"/>
       <c r="F19" s="1">
         <f>Assignment8!G19</f>
-        <v>285</v>
+        <v>435</v>
       </c>
       <c r="G19" s="1">
         <f t="shared" si="3"/>
-        <v>285</v>
+        <v>435</v>
       </c>
       <c r="H19" s="2">
         <f t="shared" si="2"/>
-        <v>0.44461778471138846</v>
+        <v>0.49097065462753953</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -16165,15 +16236,15 @@
       <c r="E20" s="8"/>
       <c r="F20" s="1">
         <f>Assignment8!G20</f>
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="G20" s="1">
         <f t="shared" si="3"/>
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="H20" s="2">
         <f t="shared" si="2"/>
-        <v>0.10920436817472699</v>
+        <v>0.12415349887133183</v>
       </c>
       <c r="J20" s="51" t="s">
         <v>43</v>
@@ -16197,15 +16268,15 @@
       <c r="E21" s="8"/>
       <c r="F21" s="1">
         <f>Assignment8!G21</f>
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="G21" s="1">
         <f t="shared" si="3"/>
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="H21" s="2">
         <f t="shared" si="2"/>
-        <v>0.1482059282371295</v>
+        <v>0.14108352144469527</v>
       </c>
       <c r="J21" s="54"/>
       <c r="K21" s="55"/>
@@ -16227,15 +16298,15 @@
       <c r="E22" s="8"/>
       <c r="F22" s="1">
         <f>Assignment8!G22</f>
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="G22" s="1">
         <f t="shared" si="3"/>
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="H22" s="2">
         <f t="shared" si="2"/>
-        <v>9.8283931357254287E-2</v>
+        <v>8.2392776523702027E-2</v>
       </c>
       <c r="J22" s="54"/>
       <c r="K22" s="55"/>
@@ -16263,11 +16334,11 @@
       </c>
       <c r="F23" s="1">
         <f>SUM(F17:F22)</f>
-        <v>641</v>
+        <v>886</v>
       </c>
       <c r="G23" s="1">
         <f>SUM(G17:G22)</f>
-        <v>641</v>
+        <v>886</v>
       </c>
       <c r="H23" s="2">
         <f>SUM(H17:H22)</f>
@@ -16338,7 +16409,7 @@
       </c>
       <c r="H26" s="2">
         <f t="shared" ref="H26:H31" si="6">IF($G$32&lt;&gt;0,G26/$G$32,"-")</f>
-        <v>5.2631578947368418E-2</v>
+        <v>0.04</v>
       </c>
       <c r="J26" s="54"/>
       <c r="K26" s="55"/>
@@ -16367,7 +16438,7 @@
       </c>
       <c r="H27" s="2">
         <f t="shared" si="6"/>
-        <v>0.10526315789473684</v>
+        <v>0.08</v>
       </c>
       <c r="J27" s="54"/>
       <c r="K27" s="55"/>
@@ -16396,7 +16467,7 @@
       </c>
       <c r="H28" s="2">
         <f t="shared" si="6"/>
-        <v>0.42105263157894735</v>
+        <v>0.32</v>
       </c>
       <c r="J28" s="57"/>
       <c r="K28" s="58"/>
@@ -16425,7 +16496,7 @@
       </c>
       <c r="H29" s="2">
         <f t="shared" si="6"/>
-        <v>0.15789473684210525</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -16437,15 +16508,15 @@
       <c r="E30" s="8"/>
       <c r="F30" s="1">
         <f>Assignment8!G30</f>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="G30" s="1">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="H30" s="2">
         <f t="shared" si="6"/>
-        <v>0.26315789473684209</v>
+        <v>0.44</v>
       </c>
       <c r="J30" s="20" t="s">
         <v>46</v>
@@ -16492,11 +16563,11 @@
       </c>
       <c r="F32" s="1">
         <f>SUM(F26:F31)</f>
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="G32" s="1">
         <f>SUM(G26:G31)</f>
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="H32" s="2">
         <f>SUM(H26:H31)</f>
@@ -16574,7 +16645,7 @@
       </c>
       <c r="H35" s="2">
         <f t="shared" ref="H35:H40" si="9">IF($G$41&lt;&gt;0,G35/$G$41,"-")</f>
-        <v>5.2631578947368418E-2</v>
+        <v>0.04</v>
       </c>
       <c r="J35" s="64"/>
       <c r="K35" s="65"/>
@@ -16603,7 +16674,7 @@
       </c>
       <c r="H36" s="2">
         <f t="shared" si="9"/>
-        <v>0.10526315789473684</v>
+        <v>0.08</v>
       </c>
       <c r="J36" s="64"/>
       <c r="K36" s="65"/>
@@ -16632,7 +16703,7 @@
       </c>
       <c r="H37" s="2">
         <f t="shared" si="9"/>
-        <v>0.42105263157894735</v>
+        <v>0.32</v>
       </c>
       <c r="J37" s="64"/>
       <c r="K37" s="65"/>
@@ -16661,7 +16732,7 @@
       </c>
       <c r="H38" s="2">
         <f t="shared" si="9"/>
-        <v>0.15789473684210525</v>
+        <v>0.12</v>
       </c>
       <c r="J38" s="64"/>
       <c r="K38" s="65"/>
@@ -16682,15 +16753,15 @@
       <c r="E39" s="8"/>
       <c r="F39" s="1">
         <f>Assignment8!G39</f>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="G39" s="1">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="H39" s="2">
         <f t="shared" si="9"/>
-        <v>0.26315789473684209</v>
+        <v>0.44</v>
       </c>
       <c r="J39" s="64"/>
       <c r="K39" s="65"/>
@@ -16743,11 +16814,11 @@
       </c>
       <c r="F41" s="1">
         <f>SUM(F35:F40)</f>
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="G41" s="1">
         <f>SUM(G35:G40)</f>
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="H41" s="2">
         <f>SUM(H35:H40)</f>

</xml_diff>